<commit_message>
update on 2024/10/9 (2)
</commit_message>
<xml_diff>
--- a/艾宾浩斯学习曲线.xlsx
+++ b/艾宾浩斯学习曲线.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="66">
   <si>
     <t>学习日期</t>
   </si>
@@ -224,6 +224,9 @@
   </si>
   <si>
     <t>数据结构1、2</t>
+  </si>
+  <si>
+    <t>三重积分</t>
   </si>
 </sst>
 </file>
@@ -1177,8 +1180,8 @@
   <sheetPr/>
   <dimension ref="A1:Q194"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="N109" sqref="N109:N110"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P11" sqref="P11:P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -3940,9 +3943,13 @@
       <c r="Q110" s="1"/>
     </row>
     <row r="111" spans="1:17">
-      <c r="A111" s="2"/>
+      <c r="A111" s="2">
+        <v>45574</v>
+      </c>
       <c r="B111" s="1"/>
-      <c r="C111" s="1"/>
+      <c r="C111" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="D111" s="1"/>
       <c r="E111" s="1"/>
       <c r="F111" s="1"/>
@@ -6409,7 +6416,6 @@
     <mergeCell ref="A101:B102"/>
     <mergeCell ref="A103:B104"/>
     <mergeCell ref="C99:I100"/>
-    <mergeCell ref="A111:B112"/>
     <mergeCell ref="A113:B114"/>
     <mergeCell ref="A115:B116"/>
     <mergeCell ref="A117:B118"/>
@@ -6498,6 +6504,7 @@
     <mergeCell ref="A105:B106"/>
     <mergeCell ref="A107:B108"/>
     <mergeCell ref="A109:B110"/>
+    <mergeCell ref="A111:B112"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>